<commit_message>
SRS updated to version 0.4
version with Mark's input and all the classes added.
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cp625\Documents\GitHub\FarmProgram\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>class</t>
   </si>
@@ -75,9 +70,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
@@ -96,10 +88,10 @@
     <t>Update Queries</t>
   </si>
   <si>
-    <t>As Forms are added</t>
-  </si>
-  <si>
     <t>Exception handling</t>
+  </si>
+  <si>
+    <t>Sanjay - Carlos</t>
   </si>
 </sst>
 </file>
@@ -243,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,7 +270,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -490,7 +482,7 @@
   <dimension ref="E2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,29 +516,29 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -557,7 +549,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -568,7 +560,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -579,7 +571,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -590,7 +582,7 @@
         <v>14</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -601,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -612,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -623,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -634,7 +626,7 @@
         <v>16</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
@@ -645,29 +637,29 @@
         <v>16</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="5:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>